<commit_message>
Se adicionan paginas y entregables
</commit_message>
<xml_diff>
--- a/src/test/resources/data/dataPrueba.xlsx
+++ b/src/test/resources/data/dataPrueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielvalenzuelasilva/IdeaProjects/IntroSelenium/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AD5F1C-4352-46D9-A89D-AA23CA522757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C725B1F5-8C00-2B48-B105-CA3BCC7B8EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{76037C72-AC24-4F08-916C-0EBDA7347AF8}"/>
+    <workbookView xWindow="33580" yWindow="5540" windowWidth="28740" windowHeight="14480" activeTab="1" xr2:uid="{76037C72-AC24-4F08-916C-0EBDA7347AF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -156,29 +156,29 @@
     <t>X</t>
   </si>
   <si>
-    <t>CP001_CREATE_ACCOUNT</t>
-  </si>
-  <si>
     <t>Domingo</t>
   </si>
   <si>
     <t>Saavedra</t>
   </si>
   <si>
-    <t>mailpruebadsasda1110001@gmail.com</t>
-  </si>
-  <si>
     <t>Tsoft1234</t>
   </si>
   <si>
     <t>Your registration completed</t>
+  </si>
+  <si>
+    <t>CP_001_Create_Account</t>
+  </si>
+  <si>
+    <t>daniedu6@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +203,14 @@
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -234,10 +242,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -247,8 +256,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -265,9 +278,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +318,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -411,7 +424,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,7 +566,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -565,7 +578,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -576,14 +589,14 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -632,28 +645,28 @@
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -938,8 +951,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{3970B86E-7D7A-DF49-B052-80BA5CF429BA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -949,7 +965,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -961,7 +977,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -973,7 +989,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>